<commit_message>
chaitanya basic scenarios add
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/Scenario1-Chaithanyaprod-TR1-Makerepayment1.xlsx
+++ b/Mifos Automation Excels/Client/Scenario1-Chaithanyaprod-TR1-Makerepayment1.xlsx
@@ -528,7 +528,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -594,7 +594,7 @@
         <v>3052.25</v>
       </c>
       <c r="F3" s="7">
-        <v>1232.8800000000001</v>
+        <v>1026.54</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -647,7 +647,7 @@
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1057,7 +1057,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
-        <v>2801</v>
+        <v>194</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>29</v>
@@ -1130,7 +1130,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
-        <v>2800</v>
+        <v>193</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>29</v>

</xml_diff>